<commit_message>
Added openpyxl to the benchmark
</commit_message>
<xml_diff>
--- a/python-test/input.xlsx
+++ b/python-test/input.xlsx
@@ -138,16 +138,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.6"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -184,27 +184,6 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="1"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="1"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="1"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="1"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="1"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="1"/>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>